<commit_message>
Updates to Data2, Data4, Data5
</commit_message>
<xml_diff>
--- a/Data2/DataDefinitions.xlsx
+++ b/Data2/DataDefinitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10425" yWindow="-195" windowWidth="27030" windowHeight="11115"/>
+    <workbookView xWindow="585" yWindow="180" windowWidth="27030" windowHeight="11115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="173">
   <si>
     <t>DataFile</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Gust from Right</t>
   </si>
   <si>
-    <t>Gust from Back</t>
-  </si>
-  <si>
     <t>Gust from Front</t>
   </si>
   <si>
@@ -439,9 +436,6 @@
     <t>2018-11-16T12:28:00.00</t>
   </si>
   <si>
-    <t>2018-11-16T12:28:57.00</t>
-  </si>
-  <si>
     <t>2018-11-16 16-29-47.csv</t>
   </si>
   <si>
@@ -539,6 +533,108 @@
   </si>
   <si>
     <t>2018-11-17T12:40:34.00</t>
+  </si>
+  <si>
+    <t>BL_2018-11-17 16-44-33.csv</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:46:02.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:46:16.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:46:09.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:46:31.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:46:59.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:47:19.00</t>
+  </si>
+  <si>
+    <t>FL_2018-11-17 16-48-51.csv</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:49:50.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:49:58.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:50:33.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:50:42.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:50:50.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:50:57.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:51:05.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:51:13.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:51:29.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:51:37.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:51:45.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:51:52.00</t>
+  </si>
+  <si>
+    <t>BR_2018-11-17 16-09-10.csv</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:41:28.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:41:36.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:41:56.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:42:07.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:42:14.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:42:22.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:42:44.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:42:51.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:43:15.00</t>
+  </si>
+  <si>
+    <t>2018-11-17T16:43:21.00</t>
+  </si>
+  <si>
+    <t>2018-11-16T12:26:00.00</t>
+  </si>
+  <si>
+    <t>2018-11-16T12:26:06.00</t>
+  </si>
+  <si>
+    <t>2018-11-16T12:27:46.00</t>
   </si>
 </sst>
 </file>
@@ -904,16 +1000,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
@@ -1032,11 +1128,11 @@
         <v>19</v>
       </c>
       <c r="J4" s="1">
-        <f>COUNTIFS(C:C,H4,D:D,$J$3)</f>
-        <v>5</v>
+        <f t="shared" ref="J4:J11" si="0">COUNTIFS(C:C,H4,D:D,$J$3)</f>
+        <v>8</v>
       </c>
       <c r="K4" s="1">
-        <f>COUNTIFS(C:C,H4,D:D,$K$3)</f>
+        <f t="shared" ref="K4:K11" si="1">COUNTIFS(C:C,H4,D:D,$K$3)</f>
         <v>2</v>
       </c>
     </row>
@@ -1051,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -1063,15 +1159,15 @@
         <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J5" s="1">
-        <f>COUNTIFS(C:C,H5,D:D,$J$3)</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="K5" s="1">
-        <f>COUNTIFS(C:C,H5,D:D,$K$3)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1100,12 +1196,12 @@
         <v>21</v>
       </c>
       <c r="J6" s="1">
-        <f>COUNTIFS(C:C,H6,D:D,$J$3)</f>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="K6" s="1">
-        <f>COUNTIFS(C:C,H6,D:D,$K$3)</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1119,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -1134,12 +1230,12 @@
         <v>22</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" ref="J7:J12" si="0">COUNTIFS(C:C,H7,D:D,$J$3)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" ref="K7:K12" si="1">COUNTIFS(C:C,H7,D:D,$K$3)</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1153,7 +1249,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1169,11 +1265,11 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1181,16 +1277,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>170</v>
       </c>
       <c r="F9">
         <v>6</v>
@@ -1215,16 +1311,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>171</v>
       </c>
       <c r="F10">
         <v>6</v>
@@ -1249,16 +1345,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -1267,15 +1363,15 @@
         <v>8</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1283,50 +1379,40 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="F12">
         <v>6</v>
       </c>
-      <c r="H12" s="3">
-        <v>9</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -1338,16 +1424,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="F14">
         <v>6</v>
@@ -1358,16 +1444,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="F15">
         <v>6</v>
@@ -1378,16 +1464,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="F16">
         <v>6</v>
@@ -1398,16 +1484,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="F17">
         <v>6</v>
@@ -1418,16 +1504,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="F18">
         <v>6</v>
@@ -1438,16 +1524,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="F19">
         <v>6</v>
@@ -1458,16 +1544,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="F20">
         <v>6</v>
@@ -1478,16 +1564,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="F21">
         <v>6</v>
@@ -1498,16 +1584,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="F22">
         <v>6</v>
@@ -1518,16 +1604,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>158</v>
       </c>
       <c r="F23">
         <v>6</v>
@@ -1538,16 +1624,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="F24">
         <v>6</v>
@@ -1558,16 +1644,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="F25">
         <v>6</v>
@@ -1578,16 +1664,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="F26">
         <v>6</v>
@@ -1598,16 +1684,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="F27">
         <v>6</v>
@@ -1618,16 +1704,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="F28">
         <v>6</v>
@@ -1638,16 +1724,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="F29">
         <v>6</v>
@@ -1658,16 +1744,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="F30">
         <v>6</v>
@@ -1678,16 +1764,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C31">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="F31">
         <v>6</v>
@@ -1698,16 +1784,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="F32">
         <v>6</v>
@@ -1718,16 +1804,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C33">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="F33">
         <v>6</v>
@@ -1738,16 +1824,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="F34">
         <v>6</v>
@@ -1758,16 +1844,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C35">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="F35">
         <v>6</v>
@@ -1778,16 +1864,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C36">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="F36">
         <v>6</v>
@@ -1798,16 +1884,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="F37">
         <v>6</v>
@@ -1818,16 +1904,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C38">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="F38">
         <v>6</v>
@@ -1838,16 +1924,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="F39">
         <v>6</v>
@@ -1858,16 +1944,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="F40">
         <v>6</v>
@@ -1878,16 +1964,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D41" t="s">
         <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="F41">
         <v>6</v>
@@ -1898,16 +1984,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="C42">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="F42">
         <v>6</v>
@@ -1918,16 +2004,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="F43">
         <v>6</v>
@@ -1938,16 +2024,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="C44">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="F44">
         <v>6</v>
@@ -1958,16 +2044,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="C45">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="F45">
         <v>6</v>
@@ -1978,16 +2064,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="C46">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="F46">
         <v>6</v>
@@ -1998,16 +2084,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="C47">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="F47">
         <v>6</v>
@@ -2018,16 +2104,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="C48">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
       <c r="F48">
         <v>6</v>
@@ -2038,16 +2124,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="C49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="F49">
         <v>6</v>
@@ -2058,16 +2144,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="C50">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="F50">
         <v>6</v>
@@ -2078,16 +2164,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="C51">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="F51">
         <v>6</v>
@@ -2098,16 +2184,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C52">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
       </c>
       <c r="E52" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="F52">
         <v>6</v>
@@ -2118,16 +2204,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C53">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
       <c r="F53">
         <v>6</v>
@@ -2138,16 +2224,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C54">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
       </c>
       <c r="E54" t="s">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="F54">
         <v>6</v>
@@ -2158,16 +2244,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C55">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="F55">
         <v>6</v>
@@ -2178,16 +2264,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C56">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="F56">
         <v>6</v>
@@ -2198,16 +2284,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C57">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
       </c>
       <c r="E57" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="F57">
         <v>6</v>
@@ -2218,16 +2304,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C58">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
       </c>
       <c r="E58" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="F58">
         <v>6</v>
@@ -2238,16 +2324,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C59">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="F59">
         <v>6</v>
@@ -2258,16 +2344,16 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C60">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D60" t="s">
         <v>6</v>
       </c>
       <c r="E60" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="F60">
         <v>6</v>
@@ -2278,16 +2364,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C61">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
       </c>
       <c r="E61" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="F61">
         <v>6</v>
@@ -2298,16 +2384,16 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C62">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D62" t="s">
         <v>6</v>
       </c>
       <c r="E62" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="F62">
         <v>6</v>
@@ -2318,16 +2404,16 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C63">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="F63">
         <v>6</v>
@@ -2338,16 +2424,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="C64">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="F64">
         <v>6</v>
@@ -2358,16 +2444,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="C65">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
       </c>
       <c r="E65" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="F65">
         <v>6</v>
@@ -2378,16 +2464,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="C66">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E66" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="F66">
         <v>6</v>
@@ -2398,16 +2484,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="C67">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D67" t="s">
         <v>6</v>
       </c>
       <c r="E67" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="F67">
         <v>6</v>
@@ -2418,16 +2504,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C68">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D68" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="F68">
         <v>6</v>
@@ -2438,16 +2524,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C69">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D69" t="s">
         <v>6</v>
       </c>
       <c r="E69" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="F69">
         <v>6</v>
@@ -2458,16 +2544,16 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C70">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D70" t="s">
         <v>6</v>
       </c>
       <c r="E70" t="s">
-        <v>91</v>
+        <v>162</v>
       </c>
       <c r="F70">
         <v>6</v>
@@ -2478,16 +2564,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C71">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E71" t="s">
-        <v>92</v>
+        <v>163</v>
       </c>
       <c r="F71">
         <v>6</v>
@@ -2498,16 +2584,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C72">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D72" t="s">
         <v>6</v>
       </c>
       <c r="E72" t="s">
-        <v>93</v>
+        <v>164</v>
       </c>
       <c r="F72">
         <v>6</v>
@@ -2518,16 +2604,16 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C73">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D73" t="s">
         <v>6</v>
       </c>
       <c r="E73" t="s">
-        <v>94</v>
+        <v>165</v>
       </c>
       <c r="F73">
         <v>6</v>
@@ -2538,16 +2624,16 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C74">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E74" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="F74">
         <v>6</v>
@@ -2558,16 +2644,16 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C75">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D75" t="s">
         <v>6</v>
       </c>
       <c r="E75" t="s">
-        <v>96</v>
+        <v>167</v>
       </c>
       <c r="F75">
         <v>6</v>
@@ -2578,16 +2664,16 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C76">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E76" t="s">
-        <v>97</v>
+        <v>168</v>
       </c>
       <c r="F76">
         <v>6</v>
@@ -2598,16 +2684,16 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
       <c r="C77">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D77" t="s">
         <v>6</v>
       </c>
       <c r="E77" t="s">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="F77">
         <v>6</v>
@@ -2618,16 +2704,16 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C78">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D78" t="s">
         <v>6</v>
       </c>
       <c r="E78" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="F78">
         <v>6</v>
@@ -2638,16 +2724,16 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C79">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D79" t="s">
         <v>6</v>
       </c>
       <c r="E79" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="F79">
         <v>6</v>
@@ -2658,16 +2744,16 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C80">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E80" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="F80">
         <v>6</v>
@@ -2678,16 +2764,16 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C81">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E81" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="F81">
         <v>6</v>
@@ -2698,16 +2784,16 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C82">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D82" t="s">
         <v>6</v>
       </c>
       <c r="E82" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="F82">
         <v>6</v>
@@ -2718,16 +2804,16 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C83">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D83" t="s">
         <v>6</v>
       </c>
       <c r="E83" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="F83">
         <v>6</v>
@@ -2738,16 +2824,16 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="C84">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D84" t="s">
         <v>6</v>
       </c>
       <c r="E84" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="F84">
         <v>6</v>
@@ -2758,16 +2844,16 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C85">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
       </c>
       <c r="E85" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="F85">
         <v>6</v>
@@ -2778,16 +2864,16 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C86">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
       </c>
       <c r="E86" t="s">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="F86">
         <v>6</v>
@@ -2798,16 +2884,16 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C87">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
       </c>
       <c r="E87" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
       <c r="F87">
         <v>6</v>
@@ -2818,16 +2904,16 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C88">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
       </c>
       <c r="E88" t="s">
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="F88">
         <v>6</v>
@@ -2838,16 +2924,16 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C89">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E89" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="F89">
         <v>6</v>
@@ -2858,16 +2944,16 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C90">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D90" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E90" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="F90">
         <v>6</v>
@@ -2878,16 +2964,16 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C91">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
       </c>
       <c r="E91" t="s">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="F91">
         <v>6</v>
@@ -2898,16 +2984,16 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
       </c>
       <c r="E92" t="s">
-        <v>116</v>
+        <v>41</v>
       </c>
       <c r="F92">
         <v>6</v>
@@ -2918,16 +3004,16 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E93" t="s">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="F93">
         <v>6</v>
@@ -2938,16 +3024,16 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C94">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
       </c>
       <c r="E94" t="s">
-        <v>118</v>
+        <v>43</v>
       </c>
       <c r="F94">
         <v>6</v>
@@ -2958,16 +3044,16 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C95">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E95" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="F95">
         <v>6</v>
@@ -2978,16 +3064,16 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C96">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D96" t="s">
         <v>6</v>
       </c>
       <c r="E96" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="F96">
         <v>6</v>
@@ -2998,16 +3084,16 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
       </c>
       <c r="E97" t="s">
-        <v>123</v>
+        <v>46</v>
       </c>
       <c r="F97">
         <v>6</v>
@@ -3018,16 +3104,16 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C98">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E98" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="F98">
         <v>6</v>
@@ -3038,16 +3124,16 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C99">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
       </c>
       <c r="E99" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="F99">
         <v>6</v>
@@ -3058,16 +3144,16 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C100">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D100" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E100" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
       <c r="F100">
         <v>6</v>
@@ -3078,16 +3164,16 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C101">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D101" t="s">
         <v>6</v>
       </c>
       <c r="E101" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
       <c r="F101">
         <v>6</v>
@@ -3098,16 +3184,16 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C102">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D102" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E102" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="F102">
         <v>6</v>
@@ -3118,16 +3204,16 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C103">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D103" t="s">
         <v>6</v>
       </c>
       <c r="E103" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="F103">
         <v>6</v>
@@ -3138,16 +3224,16 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C104">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D104" t="s">
         <v>6</v>
       </c>
       <c r="E104" t="s">
-        <v>125</v>
+        <v>53</v>
       </c>
       <c r="F104">
         <v>6</v>
@@ -3158,16 +3244,16 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C105">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D105" t="s">
         <v>6</v>
       </c>
       <c r="E105" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="F105">
         <v>6</v>
@@ -3178,16 +3264,16 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C106">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D106" t="s">
         <v>6</v>
       </c>
       <c r="E106" t="s">
-        <v>140</v>
+        <v>55</v>
       </c>
       <c r="F106">
         <v>6</v>
@@ -3198,16 +3284,16 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C107">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D107" t="s">
         <v>7</v>
       </c>
       <c r="E107" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="F107">
         <v>6</v>
@@ -3218,16 +3304,16 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C108">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D108" t="s">
         <v>6</v>
       </c>
       <c r="E108" t="s">
-        <v>132</v>
+        <v>57</v>
       </c>
       <c r="F108">
         <v>6</v>
@@ -3238,16 +3324,16 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C109">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D109" t="s">
         <v>6</v>
       </c>
       <c r="E109" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="F109">
         <v>6</v>
@@ -3258,16 +3344,16 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C110">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D110" t="s">
         <v>6</v>
       </c>
       <c r="E110" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
       <c r="F110">
         <v>6</v>
@@ -3278,16 +3364,16 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="C111">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E111" t="s">
-        <v>135</v>
+        <v>60</v>
       </c>
       <c r="F111">
         <v>6</v>
@@ -3298,16 +3384,16 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="C112">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D112" t="s">
         <v>6</v>
       </c>
       <c r="E112" t="s">
-        <v>136</v>
+        <v>62</v>
       </c>
       <c r="F112">
         <v>6</v>
@@ -3318,16 +3404,16 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="C113">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D113" t="s">
         <v>6</v>
       </c>
       <c r="E113" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="F113">
         <v>6</v>
@@ -3338,16 +3424,16 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="C114">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D114" t="s">
         <v>7</v>
       </c>
       <c r="E114" t="s">
-        <v>138</v>
+        <v>64</v>
       </c>
       <c r="F114">
         <v>6</v>
@@ -3358,18 +3444,618 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
+        <v>61</v>
+      </c>
+      <c r="C115">
+        <v>7</v>
+      </c>
+      <c r="D115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" t="s">
+        <v>65</v>
+      </c>
+      <c r="F115">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>61</v>
+      </c>
+      <c r="C116">
+        <v>7</v>
+      </c>
+      <c r="D116" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" t="s">
+        <v>66</v>
+      </c>
+      <c r="F116">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>61</v>
+      </c>
+      <c r="C117">
+        <v>7</v>
+      </c>
+      <c r="D117" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" t="s">
+        <v>67</v>
+      </c>
+      <c r="F117">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>61</v>
+      </c>
+      <c r="C118">
+        <v>7</v>
+      </c>
+      <c r="D118" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" t="s">
+        <v>68</v>
+      </c>
+      <c r="F118">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>61</v>
+      </c>
+      <c r="C119">
+        <v>7</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" t="s">
+        <v>69</v>
+      </c>
+      <c r="F119">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>61</v>
+      </c>
+      <c r="C120">
+        <v>7</v>
+      </c>
+      <c r="D120" t="s">
+        <v>7</v>
+      </c>
+      <c r="E120" t="s">
+        <v>70</v>
+      </c>
+      <c r="F120">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>61</v>
+      </c>
+      <c r="C121">
+        <v>7</v>
+      </c>
+      <c r="D121" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121" t="s">
+        <v>71</v>
+      </c>
+      <c r="F121">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>61</v>
+      </c>
+      <c r="C122">
+        <v>7</v>
+      </c>
+      <c r="D122" t="s">
+        <v>6</v>
+      </c>
+      <c r="E122" t="s">
+        <v>72</v>
+      </c>
+      <c r="F122">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>61</v>
+      </c>
+      <c r="C123">
+        <v>7</v>
+      </c>
+      <c r="D123" t="s">
+        <v>6</v>
+      </c>
+      <c r="E123" t="s">
+        <v>73</v>
+      </c>
+      <c r="F123">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>61</v>
+      </c>
+      <c r="C124">
+        <v>7</v>
+      </c>
+      <c r="D124" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124" t="s">
+        <v>74</v>
+      </c>
+      <c r="F124">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
         <v>124</v>
       </c>
-      <c r="C115">
-        <v>4</v>
-      </c>
-      <c r="D115" t="s">
-        <v>6</v>
-      </c>
-      <c r="E115" t="s">
+      <c r="B125" t="s">
+        <v>61</v>
+      </c>
+      <c r="C125">
+        <v>7</v>
+      </c>
+      <c r="D125" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" t="s">
+        <v>75</v>
+      </c>
+      <c r="F125">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>61</v>
+      </c>
+      <c r="C126">
+        <v>7</v>
+      </c>
+      <c r="D126" t="s">
+        <v>7</v>
+      </c>
+      <c r="E126" t="s">
+        <v>76</v>
+      </c>
+      <c r="F126">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>61</v>
+      </c>
+      <c r="C127">
+        <v>7</v>
+      </c>
+      <c r="D127" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" t="s">
+        <v>77</v>
+      </c>
+      <c r="F127">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>61</v>
+      </c>
+      <c r="C128">
+        <v>7</v>
+      </c>
+      <c r="D128" t="s">
+        <v>6</v>
+      </c>
+      <c r="E128" t="s">
+        <v>78</v>
+      </c>
+      <c r="F128">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>61</v>
+      </c>
+      <c r="C129">
+        <v>7</v>
+      </c>
+      <c r="D129" t="s">
+        <v>6</v>
+      </c>
+      <c r="E129" t="s">
+        <v>79</v>
+      </c>
+      <c r="F129">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>61</v>
+      </c>
+      <c r="C130">
+        <v>7</v>
+      </c>
+      <c r="D130" t="s">
+        <v>6</v>
+      </c>
+      <c r="E130" t="s">
+        <v>80</v>
+      </c>
+      <c r="F130">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>61</v>
+      </c>
+      <c r="C131">
+        <v>7</v>
+      </c>
+      <c r="D131" t="s">
+        <v>6</v>
+      </c>
+      <c r="E131" t="s">
+        <v>81</v>
+      </c>
+      <c r="F131">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>61</v>
+      </c>
+      <c r="C132">
+        <v>7</v>
+      </c>
+      <c r="D132" t="s">
+        <v>7</v>
+      </c>
+      <c r="E132" t="s">
+        <v>82</v>
+      </c>
+      <c r="F132">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>61</v>
+      </c>
+      <c r="C133">
+        <v>7</v>
+      </c>
+      <c r="D133" t="s">
+        <v>6</v>
+      </c>
+      <c r="E133" t="s">
+        <v>83</v>
+      </c>
+      <c r="F133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>84</v>
+      </c>
+      <c r="C134">
+        <v>8</v>
+      </c>
+      <c r="D134" t="s">
+        <v>6</v>
+      </c>
+      <c r="E134" t="s">
+        <v>85</v>
+      </c>
+      <c r="F134">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>84</v>
+      </c>
+      <c r="C135">
+        <v>8</v>
+      </c>
+      <c r="D135" t="s">
+        <v>6</v>
+      </c>
+      <c r="E135" t="s">
+        <v>86</v>
+      </c>
+      <c r="F135">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>84</v>
+      </c>
+      <c r="C136">
+        <v>8</v>
+      </c>
+      <c r="D136" t="s">
+        <v>6</v>
+      </c>
+      <c r="E136" t="s">
+        <v>87</v>
+      </c>
+      <c r="F136">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>84</v>
+      </c>
+      <c r="C137">
+        <v>8</v>
+      </c>
+      <c r="D137" t="s">
+        <v>6</v>
+      </c>
+      <c r="E137" t="s">
+        <v>88</v>
+      </c>
+      <c r="F137">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>84</v>
+      </c>
+      <c r="C138">
+        <v>8</v>
+      </c>
+      <c r="D138" t="s">
+        <v>7</v>
+      </c>
+      <c r="E138" t="s">
+        <v>89</v>
+      </c>
+      <c r="F138">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>84</v>
+      </c>
+      <c r="C139">
+        <v>8</v>
+      </c>
+      <c r="D139" t="s">
+        <v>6</v>
+      </c>
+      <c r="E139" t="s">
+        <v>90</v>
+      </c>
+      <c r="F139">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
         <v>139</v>
       </c>
-      <c r="F115">
+      <c r="B140" t="s">
+        <v>84</v>
+      </c>
+      <c r="C140">
+        <v>8</v>
+      </c>
+      <c r="D140" t="s">
+        <v>6</v>
+      </c>
+      <c r="E140" t="s">
+        <v>91</v>
+      </c>
+      <c r="F140">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>84</v>
+      </c>
+      <c r="C141">
+        <v>8</v>
+      </c>
+      <c r="D141" t="s">
+        <v>6</v>
+      </c>
+      <c r="E141" t="s">
+        <v>92</v>
+      </c>
+      <c r="F141">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>84</v>
+      </c>
+      <c r="C142">
+        <v>8</v>
+      </c>
+      <c r="D142" t="s">
+        <v>6</v>
+      </c>
+      <c r="E142" t="s">
+        <v>93</v>
+      </c>
+      <c r="F142">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>84</v>
+      </c>
+      <c r="C143">
+        <v>8</v>
+      </c>
+      <c r="D143" t="s">
+        <v>6</v>
+      </c>
+      <c r="E143" t="s">
+        <v>94</v>
+      </c>
+      <c r="F143">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>84</v>
+      </c>
+      <c r="C144">
+        <v>8</v>
+      </c>
+      <c r="D144" t="s">
+        <v>7</v>
+      </c>
+      <c r="E144" t="s">
+        <v>95</v>
+      </c>
+      <c r="F144">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>84</v>
+      </c>
+      <c r="C145">
+        <v>8</v>
+      </c>
+      <c r="D145" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" t="s">
+        <v>96</v>
+      </c>
+      <c r="F145">
         <v>6</v>
       </c>
     </row>

</xml_diff>